<commit_message>
Se agrega codigo de la ReLU
</commit_message>
<xml_diff>
--- a/BatchNormalization/EntendiendoBN.xlsx
+++ b/BatchNormalization/EntendiendoBN.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Embedded_AI\ImplementacionCapas\LayersImplementationsCNN\PythonImplementations\BatchNormalization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Embedded_AI\ImplementacionCapas\LayersImplementationsCNN\BatchNormalization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A2B412-7462-4DD4-99BE-945262EB5EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2389D42-8ADC-49D1-B2B1-B79492AF7F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13455" xr2:uid="{E907E16A-777B-4A63-B53D-C1F88FE012E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="9840" windowHeight="8790" activeTab="1" xr2:uid="{E907E16A-777B-4A63-B53D-C1F88FE012E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lineal" sheetId="1" r:id="rId1"/>
+    <sheet name="Matriz 3x4x4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Voltaje X</t>
   </si>
@@ -61,6 +62,27 @@
   </si>
   <si>
     <t>Beta</t>
+  </si>
+  <si>
+    <t>Matriz 1</t>
+  </si>
+  <si>
+    <t>Matriz 2</t>
+  </si>
+  <si>
+    <t>Matriz 3</t>
+  </si>
+  <si>
+    <t>Matriz 1 Norm</t>
+  </si>
+  <si>
+    <t>Matriz 2 Norm</t>
+  </si>
+  <si>
+    <t>Matriz 3 Norm</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -68,12 +90,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,10 +142,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64651440-1B3A-43A4-9CB1-E7E49E20E1AB}">
   <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="D13:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +622,7 @@
         <v>0.68728358762019326</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="2"/>
+        <f>(C10-$C$15)^2</f>
         <v>1</v>
       </c>
     </row>
@@ -600,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
+        <f>(C11-$C$15)/(SQRT($C$16+$C$17))</f>
         <v>0.94868329805051377</v>
       </c>
       <c r="F11" s="2">
@@ -642,7 +673,7 @@
         <v>1.3117936440504832</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="2"/>
+        <f>(C13-$C$15)^2</f>
         <v>6.25</v>
       </c>
     </row>
@@ -696,4 +727,635 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787523A0-41BB-486C-A6C6-8745A733C364}">
+  <dimension ref="B2:M21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3">
+        <f>(H3-$H$19)/(SQRT($H$20+H21))</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J3" s="3">
+        <v>8</v>
+      </c>
+      <c r="K3" s="3">
+        <f>(J3-$J$19)/(SQRT($J$20+J21))</f>
+        <v>0.84119102419205982</v>
+      </c>
+      <c r="L3" s="3">
+        <v>5</v>
+      </c>
+      <c r="M3" s="3">
+        <f>(L3-$L$19)/(SQRT($L$20+L21))</f>
+        <v>-9.8532927816429319E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I18" si="0">(H4-$H$19)/(SQRT($H$20+H22))</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J4" s="3">
+        <v>5</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K18" si="1">(J4-$J$19)/(SQRT($J$20+J22))</f>
+        <v>-7.6471911290187253E-2</v>
+      </c>
+      <c r="L4" s="3">
+        <v>6</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M18" si="2">(L4-$L$19)/(SQRT($L$20+L22))</f>
+        <v>0.29559878344928797</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3">
+        <v>6</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J5" s="3">
+        <v>5</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>-7.6471911290187253E-2</v>
+      </c>
+      <c r="L5" s="3">
+        <v>6</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.29559878344928797</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H6" s="3">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J6" s="3">
+        <v>8</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.84119102419205982</v>
+      </c>
+      <c r="L6" s="3">
+        <v>5</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="2"/>
+        <v>-9.8532927816429319E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8</v>
+      </c>
+      <c r="H7" s="3">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J7" s="3">
+        <v>8</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.84119102419205982</v>
+      </c>
+      <c r="L7" s="3">
+        <v>8</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0838622059807226</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.7320508075688774</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>-1.6059101370939324</v>
+      </c>
+      <c r="L8" s="3">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.2809280616135812</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.7320508075688774</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>-1.6059101370939324</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.6750597728792984</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3">
+        <v>6</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J10" s="3">
+        <v>8</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.84119102419205982</v>
+      </c>
+      <c r="L10" s="3">
+        <v>9</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4779939172464398</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H11" s="3">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J11" s="3">
+        <v>8</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.84119102419205982</v>
+      </c>
+      <c r="L11" s="3">
+        <v>9</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4779939172464398</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.7320508075688774</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>-1.6059101370939324</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.6750597728792984</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>9</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="0"/>
+        <v>-1.7320508075688774</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="1"/>
+        <v>-1.6059101370939324</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.2809280616135812</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>8</v>
+      </c>
+      <c r="H14" s="3">
+        <v>6</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J14" s="3">
+        <v>8</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>0.84119102419205982</v>
+      </c>
+      <c r="L14" s="3">
+        <v>8</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0838622059807226</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>6</v>
+      </c>
+      <c r="H15" s="3">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J15" s="3">
+        <v>8</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.84119102419205982</v>
+      </c>
+      <c r="L15" s="3">
+        <v>6</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="2"/>
+        <v>0.29559878344928797</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H16" s="3">
+        <v>6</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J16" s="3">
+        <v>5</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>-7.6471911290187253E-2</v>
+      </c>
+      <c r="L16" s="3">
+        <v>5</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="2"/>
+        <v>-9.8532927816429319E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H17" s="3">
+        <v>6</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J17" s="3">
+        <v>5</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="1"/>
+        <v>-7.6471911290187253E-2</v>
+      </c>
+      <c r="L17" s="3">
+        <v>5</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="2"/>
+        <v>-9.8532927816429319E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H18" s="3">
+        <v>6</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="J18" s="3">
+        <v>8</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="1"/>
+        <v>0.84119102419205982</v>
+      </c>
+      <c r="L18" s="3">
+        <v>6</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="2"/>
+        <v>0.29559878344928797</v>
+      </c>
+    </row>
+    <row r="19" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <f>AVERAGE(H3:H18)</f>
+        <v>5</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="3">
+        <f>AVERAGE(J3:J18)</f>
+        <v>5.25</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="3">
+        <f>AVERAGE(L3:L18)</f>
+        <v>5.25</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3">
+        <f>((H3-H19)^2+(H4-H19)^2+(H5-H19)^2+(H6-H19)^2+(H7-H19)^2+(H8-H19)^2+(H9-H19)^2+(H10-H19)^2+(H11-H19)^2+(H12-H19)^2+(H13-H19)^2+(H14-H19)^2+(H15-H19)^2+(H16-H19)^2+(H17-H19)^2+(H18-H19)^2)/16</f>
+        <v>3</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" ref="I20:J20" si="3">((J3-J19)^2+(J4-J19)^2+(J5-J19)^2+(J6-J19)^2+(J7-J19)^2+(J8-J19)^2+(J9-J19)^2+(J10-J19)^2+(J11-J19)^2+(J12-J19)^2+(J13-J19)^2+(J14-J19)^2+(J15-J19)^2+(J16-J19)^2+(J17-J19)^2+(J18-J19)^2)/16</f>
+        <v>10.6875</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" ref="L20" si="4">((L3-L19)^2+(L4-L19)^2+(L5-L19)^2+(L6-L19)^2+(L7-L19)^2+(L8-L19)^2+(L9-L19)^2+(L10-L19)^2+(L11-L19)^2+(L12-L19)^2+(L13-L19)^2+(L14-L19)^2+(L15-L19)^2+(L16-L19)^2+(L17-L19)^2+(L18-L19)^2)/16</f>
+        <v>6.4375</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>